<commit_message>
Updated Metrics Document and Sprint Backlog
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint1/Sprint Backlog.xlsx
+++ b/Project/Phase 2/Sprint1/Sprint Backlog.xlsx
@@ -5,18 +5,29 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AntiMach\Desktop\uni-workspace\ES\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pmtbl\Documents\GitHub\SE2223_57514_60045_60602_60694_60700\Project\Phase 2\Sprint1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E05D50-7DBA-420B-BAB3-AB5661C4E60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407AE6F2-CC8B-40FE-8AD5-6D333DBE7C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7migQJ+lrbl2DYfX+I5gs2U1BecDZA=="/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>TODO</t>
   </si>
@@ -56,16 +67,37 @@
   <si>
     <t>Pedro Lopes</t>
   </si>
+  <si>
+    <t>Collect Metrics
+Explain Metrics collected
+Find potencial trouble spots
+Try and relate metrics with code smells</t>
+  </si>
+  <si>
+    <t>Find potencial trouble spots
+Try and relate metrics with code smells</t>
+  </si>
+  <si>
+    <t>Collect Metrics
+Explain Metrics collected</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -87,7 +119,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +162,54 @@
         <bgColor rgb="FFFFE598"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFC9696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFC9696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFC9696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFC9696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -165,49 +245,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -426,7 +526,7 @@
   <dimension ref="B1:K1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:G3"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -447,139 +547,151 @@
   <sheetData>
     <row r="1" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="9"/>
+      <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="16" t="s">
+      <c r="G2" s="9"/>
+      <c r="H2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="16"/>
-      <c r="K2" s="10" t="s">
+      <c r="I2" s="11"/>
+      <c r="K2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="K3" s="11" t="s">
+      <c r="B3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="K3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="3"/>
-      <c r="K4" s="12" t="s">
+      <c r="B4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="9"/>
+      <c r="K4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="7"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="3"/>
-      <c r="K5" s="13" t="s">
+      <c r="B5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="9"/>
+      <c r="K5" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="3"/>
-      <c r="K6" s="14" t="s">
+      <c r="B6" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="19"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="9"/>
+      <c r="K6" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="3"/>
+      <c r="B7" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="9"/>
       <c r="J7" s="1"/>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="7" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
     </row>
     <row r="10" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
     </row>
     <row r="11" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
     </row>
     <row r="12" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1572,21 +1684,6 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="F7:G7"/>
     <mergeCell ref="F6:G6"/>
@@ -1596,6 +1693,21 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="F3:G3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>